<commit_message>
added vercel.json for route issue
</commit_message>
<xml_diff>
--- a/src/data/flash-dsa-data.xlsx
+++ b/src/data/flash-dsa-data.xlsx
@@ -8194,7 +8194,7 @@
     <xf numFmtId="42" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
     <xf numFmtId="9" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
   </cellStyleXfs>
-  <cellXfs count="6">
+  <cellXfs count="4">
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="false" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
@@ -8208,14 +8208,6 @@
       <protection locked="true" hidden="false"/>
     </xf>
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="true">
-      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
-    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
-      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
-    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
@@ -8239,13 +8231,13 @@
   <dimension ref="A1:I418"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="120" zoomScaleNormal="120" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="B14" activeCellId="0" sqref="B14"/>
+      <selection pane="topLeft" activeCell="D14" activeCellId="0" sqref="D14"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.54296875" defaultRowHeight="13.5" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="1" width="45.74"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="4" min="4" style="1" width="63.69"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="4" min="4" style="1" width="63.7"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="8" min="8" style="1" width="19.84"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="9" min="9" style="1" width="35.98"/>
   </cols>
@@ -10413,7 +10405,7 @@
       <c r="C89" s="1" t="s">
         <v>377</v>
       </c>
-      <c r="D89" s="4" t="s">
+      <c r="D89" s="2" t="s">
         <v>378</v>
       </c>
       <c r="E89" s="1" t="s">
@@ -10439,7 +10431,7 @@
       <c r="C90" s="1" t="s">
         <v>383</v>
       </c>
-      <c r="D90" s="4" t="s">
+      <c r="D90" s="2" t="s">
         <v>384</v>
       </c>
       <c r="E90" s="1" t="s">
@@ -10463,7 +10455,7 @@
       <c r="C91" s="1" t="s">
         <v>387</v>
       </c>
-      <c r="D91" s="4" t="s">
+      <c r="D91" s="2" t="s">
         <v>388</v>
       </c>
       <c r="E91" s="1" t="s">
@@ -10489,7 +10481,7 @@
       <c r="C92" s="1" t="s">
         <v>392</v>
       </c>
-      <c r="D92" s="4" t="s">
+      <c r="D92" s="2" t="s">
         <v>393</v>
       </c>
       <c r="E92" s="1" t="s">
@@ -10513,7 +10505,7 @@
       <c r="C93" s="1" t="s">
         <v>396</v>
       </c>
-      <c r="D93" s="4" t="s">
+      <c r="D93" s="2" t="s">
         <v>397</v>
       </c>
       <c r="E93" s="1" t="s">
@@ -10537,7 +10529,7 @@
       <c r="C94" s="1" t="s">
         <v>400</v>
       </c>
-      <c r="D94" s="4" t="s">
+      <c r="D94" s="2" t="s">
         <v>401</v>
       </c>
       <c r="E94" s="1" t="s">
@@ -10561,7 +10553,7 @@
       <c r="C95" s="1" t="s">
         <v>404</v>
       </c>
-      <c r="D95" s="4" t="s">
+      <c r="D95" s="2" t="s">
         <v>405</v>
       </c>
       <c r="E95" s="1" t="s">
@@ -10585,7 +10577,7 @@
       <c r="C96" s="1" t="s">
         <v>408</v>
       </c>
-      <c r="D96" s="4" t="s">
+      <c r="D96" s="2" t="s">
         <v>409</v>
       </c>
       <c r="E96" s="1" t="s">
@@ -10609,7 +10601,7 @@
       <c r="C97" s="1" t="s">
         <v>412</v>
       </c>
-      <c r="D97" s="4" t="s">
+      <c r="D97" s="2" t="s">
         <v>413</v>
       </c>
       <c r="E97" s="1" t="s">
@@ -10633,7 +10625,7 @@
       <c r="C98" s="1" t="s">
         <v>416</v>
       </c>
-      <c r="D98" s="4" t="s">
+      <c r="D98" s="2" t="s">
         <v>417</v>
       </c>
       <c r="E98" s="1" t="s">
@@ -10657,7 +10649,7 @@
       <c r="C99" s="1" t="s">
         <v>420</v>
       </c>
-      <c r="D99" s="4" t="s">
+      <c r="D99" s="2" t="s">
         <v>421</v>
       </c>
       <c r="E99" s="1" t="s">
@@ -10681,7 +10673,7 @@
       <c r="C100" s="1" t="s">
         <v>420</v>
       </c>
-      <c r="D100" s="4" t="s">
+      <c r="D100" s="2" t="s">
         <v>421</v>
       </c>
       <c r="E100" s="1" t="s">
@@ -10707,7 +10699,7 @@
       <c r="C101" s="1" t="s">
         <v>427</v>
       </c>
-      <c r="D101" s="4" t="s">
+      <c r="D101" s="2" t="s">
         <v>428</v>
       </c>
       <c r="E101" s="1" t="s">
@@ -10733,7 +10725,7 @@
       <c r="C102" s="1" t="s">
         <v>432</v>
       </c>
-      <c r="D102" s="4" t="s">
+      <c r="D102" s="2" t="s">
         <v>433</v>
       </c>
       <c r="E102" s="1" t="s">
@@ -10759,7 +10751,7 @@
       <c r="C103" s="1" t="s">
         <v>437</v>
       </c>
-      <c r="D103" s="4" t="s">
+      <c r="D103" s="2" t="s">
         <v>438</v>
       </c>
       <c r="E103" s="1" t="s">
@@ -10783,7 +10775,7 @@
       <c r="C104" s="1" t="s">
         <v>441</v>
       </c>
-      <c r="D104" s="4" t="s">
+      <c r="D104" s="2" t="s">
         <v>442</v>
       </c>
       <c r="E104" s="1" t="s">
@@ -10809,7 +10801,7 @@
       <c r="C105" s="1" t="s">
         <v>446</v>
       </c>
-      <c r="D105" s="4" t="s">
+      <c r="D105" s="2" t="s">
         <v>447</v>
       </c>
       <c r="E105" s="1" t="s">
@@ -10835,7 +10827,7 @@
       <c r="C106" s="1" t="s">
         <v>451</v>
       </c>
-      <c r="D106" s="4" t="s">
+      <c r="D106" s="2" t="s">
         <v>452</v>
       </c>
       <c r="E106" s="1" t="s">
@@ -10861,7 +10853,7 @@
       <c r="C107" s="1" t="s">
         <v>456</v>
       </c>
-      <c r="D107" s="4" t="s">
+      <c r="D107" s="2" t="s">
         <v>457</v>
       </c>
       <c r="E107" s="1" t="s">
@@ -10887,7 +10879,7 @@
       <c r="C108" s="1" t="s">
         <v>461</v>
       </c>
-      <c r="D108" s="4" t="s">
+      <c r="D108" s="2" t="s">
         <v>462</v>
       </c>
       <c r="E108" s="1" t="s">
@@ -10913,7 +10905,7 @@
       <c r="C109" s="1" t="s">
         <v>466</v>
       </c>
-      <c r="D109" s="4" t="s">
+      <c r="D109" s="2" t="s">
         <v>467</v>
       </c>
       <c r="E109" s="1" t="s">
@@ -10939,7 +10931,7 @@
       <c r="C110" s="1" t="s">
         <v>471</v>
       </c>
-      <c r="D110" s="4" t="s">
+      <c r="D110" s="2" t="s">
         <v>472</v>
       </c>
       <c r="E110" s="1" t="s">
@@ -10965,7 +10957,7 @@
       <c r="C111" s="1" t="s">
         <v>476</v>
       </c>
-      <c r="D111" s="4" t="s">
+      <c r="D111" s="2" t="s">
         <v>477</v>
       </c>
       <c r="E111" s="1" t="s">
@@ -10991,7 +10983,7 @@
       <c r="C112" s="1" t="s">
         <v>481</v>
       </c>
-      <c r="D112" s="4" t="s">
+      <c r="D112" s="2" t="s">
         <v>482</v>
       </c>
       <c r="E112" s="1" t="s">
@@ -11017,7 +11009,7 @@
       <c r="C113" s="1" t="s">
         <v>486</v>
       </c>
-      <c r="D113" s="4" t="s">
+      <c r="D113" s="2" t="s">
         <v>487</v>
       </c>
       <c r="E113" s="1" t="s">
@@ -11043,7 +11035,7 @@
       <c r="C114" s="1" t="s">
         <v>491</v>
       </c>
-      <c r="D114" s="4" t="s">
+      <c r="D114" s="2" t="s">
         <v>492</v>
       </c>
       <c r="E114" s="1" t="s">
@@ -11069,7 +11061,7 @@
       <c r="C115" s="1" t="s">
         <v>496</v>
       </c>
-      <c r="D115" s="4" t="s">
+      <c r="D115" s="2" t="s">
         <v>497</v>
       </c>
       <c r="E115" s="1" t="s">
@@ -11095,7 +11087,7 @@
       <c r="C116" s="1" t="s">
         <v>501</v>
       </c>
-      <c r="D116" s="4" t="s">
+      <c r="D116" s="2" t="s">
         <v>502</v>
       </c>
       <c r="E116" s="1" t="s">
@@ -11121,7 +11113,7 @@
       <c r="C117" s="1" t="s">
         <v>506</v>
       </c>
-      <c r="D117" s="4" t="s">
+      <c r="D117" s="2" t="s">
         <v>507</v>
       </c>
       <c r="E117" s="1" t="s">
@@ -11147,7 +11139,7 @@
       <c r="C118" s="1" t="s">
         <v>511</v>
       </c>
-      <c r="D118" s="4" t="s">
+      <c r="D118" s="2" t="s">
         <v>512</v>
       </c>
       <c r="E118" s="1" t="s">
@@ -11173,7 +11165,7 @@
       <c r="C119" s="1" t="s">
         <v>516</v>
       </c>
-      <c r="D119" s="4" t="s">
+      <c r="D119" s="2" t="s">
         <v>517</v>
       </c>
       <c r="E119" s="1" t="s">
@@ -11197,7 +11189,7 @@
       <c r="C120" s="1" t="s">
         <v>368</v>
       </c>
-      <c r="D120" s="4" t="s">
+      <c r="D120" s="2" t="s">
         <v>520</v>
       </c>
       <c r="E120" s="1" t="s">
@@ -11223,7 +11215,7 @@
       <c r="C121" s="1" t="s">
         <v>525</v>
       </c>
-      <c r="D121" s="4" t="s">
+      <c r="D121" s="2" t="s">
         <v>526</v>
       </c>
       <c r="E121" s="1" t="s">
@@ -11249,7 +11241,7 @@
       <c r="C122" s="1" t="s">
         <v>530</v>
       </c>
-      <c r="D122" s="4" t="s">
+      <c r="D122" s="2" t="s">
         <v>531</v>
       </c>
       <c r="E122" s="1" t="s">
@@ -11275,7 +11267,7 @@
       <c r="C123" s="1" t="s">
         <v>535</v>
       </c>
-      <c r="D123" s="4" t="s">
+      <c r="D123" s="2" t="s">
         <v>536</v>
       </c>
       <c r="E123" s="1" t="s">
@@ -11301,7 +11293,7 @@
       <c r="C124" s="1" t="s">
         <v>540</v>
       </c>
-      <c r="D124" s="4" t="s">
+      <c r="D124" s="2" t="s">
         <v>541</v>
       </c>
       <c r="E124" s="1" t="s">
@@ -11327,7 +11319,7 @@
       <c r="C125" s="1" t="s">
         <v>545</v>
       </c>
-      <c r="D125" s="4" t="s">
+      <c r="D125" s="2" t="s">
         <v>546</v>
       </c>
       <c r="E125" s="1" t="s">
@@ -11353,7 +11345,7 @@
       <c r="C126" s="1" t="s">
         <v>550</v>
       </c>
-      <c r="D126" s="4" t="s">
+      <c r="D126" s="2" t="s">
         <v>551</v>
       </c>
       <c r="E126" s="1" t="s">
@@ -11379,7 +11371,7 @@
       <c r="C127" s="1" t="s">
         <v>555</v>
       </c>
-      <c r="D127" s="4" t="s">
+      <c r="D127" s="2" t="s">
         <v>556</v>
       </c>
       <c r="E127" s="1" t="s">
@@ -11405,7 +11397,7 @@
       <c r="C128" s="1" t="s">
         <v>560</v>
       </c>
-      <c r="D128" s="4" t="s">
+      <c r="D128" s="2" t="s">
         <v>561</v>
       </c>
       <c r="E128" s="1" t="s">
@@ -11431,7 +11423,7 @@
       <c r="C129" s="1" t="s">
         <v>565</v>
       </c>
-      <c r="D129" s="4" t="s">
+      <c r="D129" s="2" t="s">
         <v>566</v>
       </c>
       <c r="E129" s="1" t="s">
@@ -11457,7 +11449,7 @@
       <c r="C130" s="1" t="s">
         <v>570</v>
       </c>
-      <c r="D130" s="4" t="s">
+      <c r="D130" s="2" t="s">
         <v>571</v>
       </c>
       <c r="E130" s="1" t="s">
@@ -11483,7 +11475,7 @@
       <c r="C131" s="1" t="s">
         <v>575</v>
       </c>
-      <c r="D131" s="4" t="s">
+      <c r="D131" s="2" t="s">
         <v>576</v>
       </c>
       <c r="E131" s="1" t="s">
@@ -11509,7 +11501,7 @@
       <c r="C132" s="1" t="s">
         <v>580</v>
       </c>
-      <c r="D132" s="4" t="s">
+      <c r="D132" s="2" t="s">
         <v>581</v>
       </c>
       <c r="E132" s="1" t="s">
@@ -11535,7 +11527,7 @@
       <c r="C133" s="1" t="s">
         <v>585</v>
       </c>
-      <c r="D133" s="4" t="s">
+      <c r="D133" s="2" t="s">
         <v>586</v>
       </c>
       <c r="E133" s="1" t="s">
@@ -11561,7 +11553,7 @@
       <c r="C134" s="1" t="s">
         <v>590</v>
       </c>
-      <c r="D134" s="4" t="s">
+      <c r="D134" s="2" t="s">
         <v>591</v>
       </c>
       <c r="E134" s="1" t="s">
@@ -11587,7 +11579,7 @@
       <c r="C135" s="1" t="s">
         <v>595</v>
       </c>
-      <c r="D135" s="4" t="s">
+      <c r="D135" s="2" t="s">
         <v>596</v>
       </c>
       <c r="E135" s="1" t="s">
@@ -11613,7 +11605,7 @@
       <c r="C136" s="1" t="s">
         <v>600</v>
       </c>
-      <c r="D136" s="4" t="s">
+      <c r="D136" s="2" t="s">
         <v>601</v>
       </c>
       <c r="E136" s="1" t="s">
@@ -11635,7 +11627,7 @@
       <c r="C137" s="1" t="s">
         <v>603</v>
       </c>
-      <c r="D137" s="4" t="s">
+      <c r="D137" s="2" t="s">
         <v>604</v>
       </c>
       <c r="E137" s="1" t="s">
@@ -11661,7 +11653,7 @@
       <c r="C138" s="1" t="s">
         <v>608</v>
       </c>
-      <c r="D138" s="4" t="s">
+      <c r="D138" s="2" t="s">
         <v>609</v>
       </c>
       <c r="E138" s="1" t="s">
@@ -11687,7 +11679,7 @@
       <c r="C139" s="1" t="s">
         <v>613</v>
       </c>
-      <c r="D139" s="4" t="s">
+      <c r="D139" s="2" t="s">
         <v>614</v>
       </c>
       <c r="E139" s="1" t="s">
@@ -11713,7 +11705,7 @@
       <c r="C140" s="1" t="s">
         <v>618</v>
       </c>
-      <c r="D140" s="4" t="s">
+      <c r="D140" s="2" t="s">
         <v>619</v>
       </c>
       <c r="E140" s="1" t="s">
@@ -11739,7 +11731,7 @@
       <c r="C141" s="1" t="s">
         <v>623</v>
       </c>
-      <c r="D141" s="4" t="s">
+      <c r="D141" s="2" t="s">
         <v>624</v>
       </c>
       <c r="E141" s="1" t="s">
@@ -11765,7 +11757,7 @@
       <c r="C142" s="1" t="s">
         <v>628</v>
       </c>
-      <c r="D142" s="4" t="s">
+      <c r="D142" s="2" t="s">
         <v>629</v>
       </c>
       <c r="E142" s="1" t="s">
@@ -11787,7 +11779,7 @@
       <c r="C143" s="1" t="s">
         <v>631</v>
       </c>
-      <c r="D143" s="4" t="s">
+      <c r="D143" s="2" t="s">
         <v>632</v>
       </c>
       <c r="E143" s="1" t="s">
@@ -11813,7 +11805,7 @@
       <c r="C144" s="1" t="s">
         <v>636</v>
       </c>
-      <c r="D144" s="4" t="s">
+      <c r="D144" s="2" t="s">
         <v>637</v>
       </c>
       <c r="E144" s="1" t="s">
@@ -13375,7 +13367,7 @@
       <c r="C222" s="1" t="s">
         <v>794</v>
       </c>
-      <c r="D222" s="4" t="s">
+      <c r="D222" s="2" t="s">
         <v>795</v>
       </c>
       <c r="E222" s="1" t="s">
@@ -13401,7 +13393,7 @@
       <c r="C223" s="1" t="s">
         <v>800</v>
       </c>
-      <c r="D223" s="4" t="s">
+      <c r="D223" s="2" t="s">
         <v>801</v>
       </c>
       <c r="E223" s="1" t="s">
@@ -13427,7 +13419,7 @@
       <c r="C224" s="1" t="s">
         <v>805</v>
       </c>
-      <c r="D224" s="4" t="s">
+      <c r="D224" s="2" t="s">
         <v>806</v>
       </c>
       <c r="E224" s="1" t="s">
@@ -13453,7 +13445,7 @@
       <c r="C225" s="1" t="s">
         <v>810</v>
       </c>
-      <c r="D225" s="4" t="s">
+      <c r="D225" s="2" t="s">
         <v>811</v>
       </c>
       <c r="E225" s="1" t="s">
@@ -13479,7 +13471,7 @@
       <c r="C226" s="1" t="s">
         <v>815</v>
       </c>
-      <c r="D226" s="4" t="s">
+      <c r="D226" s="2" t="s">
         <v>816</v>
       </c>
       <c r="E226" s="1" t="s">
@@ -13505,7 +13497,7 @@
       <c r="C227" s="1" t="s">
         <v>820</v>
       </c>
-      <c r="D227" s="4" t="s">
+      <c r="D227" s="2" t="s">
         <v>821</v>
       </c>
       <c r="E227" s="1" t="s">
@@ -13531,7 +13523,7 @@
       <c r="C228" s="1" t="s">
         <v>825</v>
       </c>
-      <c r="D228" s="4" t="s">
+      <c r="D228" s="2" t="s">
         <v>826</v>
       </c>
       <c r="E228" s="1" t="s">
@@ -13557,7 +13549,7 @@
       <c r="C229" s="1" t="s">
         <v>830</v>
       </c>
-      <c r="D229" s="4" t="s">
+      <c r="D229" s="2" t="s">
         <v>831</v>
       </c>
       <c r="E229" s="1" t="s">
@@ -13579,7 +13571,7 @@
       <c r="C230" s="1" t="s">
         <v>833</v>
       </c>
-      <c r="D230" s="4" t="s">
+      <c r="D230" s="2" t="s">
         <v>834</v>
       </c>
       <c r="E230" s="1" t="s">
@@ -13605,7 +13597,7 @@
       <c r="C231" s="1" t="s">
         <v>838</v>
       </c>
-      <c r="D231" s="4" t="s">
+      <c r="D231" s="2" t="s">
         <v>839</v>
       </c>
       <c r="E231" s="1" t="s">
@@ -13631,7 +13623,7 @@
       <c r="C232" s="1" t="s">
         <v>843</v>
       </c>
-      <c r="D232" s="4" t="s">
+      <c r="D232" s="2" t="s">
         <v>844</v>
       </c>
       <c r="E232" s="1" t="s">
@@ -13657,7 +13649,7 @@
       <c r="C233" s="1" t="s">
         <v>848</v>
       </c>
-      <c r="D233" s="4" t="s">
+      <c r="D233" s="2" t="s">
         <v>849</v>
       </c>
       <c r="E233" s="1" t="s">
@@ -13679,7 +13671,6 @@
       <c r="C234" s="1" t="s">
         <v>851</v>
       </c>
-      <c r="D234" s="0"/>
       <c r="E234" s="1" t="s">
         <v>796</v>
       </c>
@@ -13697,7 +13688,7 @@
       <c r="C235" s="1" t="s">
         <v>853</v>
       </c>
-      <c r="D235" s="4" t="s">
+      <c r="D235" s="2" t="s">
         <v>854</v>
       </c>
       <c r="E235" s="1" t="s">
@@ -13723,7 +13714,7 @@
       <c r="C236" s="1" t="s">
         <v>163</v>
       </c>
-      <c r="D236" s="4" t="s">
+      <c r="D236" s="2" t="s">
         <v>858</v>
       </c>
       <c r="E236" s="1" t="s">
@@ -13749,7 +13740,7 @@
       <c r="C237" s="1" t="s">
         <v>862</v>
       </c>
-      <c r="D237" s="4" t="s">
+      <c r="D237" s="2" t="s">
         <v>863</v>
       </c>
       <c r="E237" s="1" t="s">
@@ -13775,7 +13766,7 @@
       <c r="C238" s="1" t="s">
         <v>867</v>
       </c>
-      <c r="D238" s="4" t="s">
+      <c r="D238" s="2" t="s">
         <v>868</v>
       </c>
       <c r="E238" s="1" t="s">
@@ -13799,7 +13790,7 @@
       <c r="C239" s="1" t="s">
         <v>872</v>
       </c>
-      <c r="D239" s="4" t="s">
+      <c r="D239" s="2" t="s">
         <v>873</v>
       </c>
       <c r="E239" s="1" t="s">
@@ -13825,7 +13816,7 @@
       <c r="C240" s="1" t="s">
         <v>872</v>
       </c>
-      <c r="D240" s="4" t="s">
+      <c r="D240" s="2" t="s">
         <v>3</v>
       </c>
       <c r="E240" s="1" t="s">
@@ -13849,7 +13840,7 @@
       <c r="C241" s="1" t="s">
         <v>879</v>
       </c>
-      <c r="D241" s="4" t="s">
+      <c r="D241" s="2" t="s">
         <v>880</v>
       </c>
       <c r="E241" s="1" t="s">
@@ -13875,7 +13866,7 @@
       <c r="C242" s="1" t="s">
         <v>884</v>
       </c>
-      <c r="D242" s="4" t="s">
+      <c r="D242" s="2" t="s">
         <v>885</v>
       </c>
       <c r="E242" s="1" t="s">
@@ -13899,7 +13890,7 @@
       <c r="C243" s="1" t="s">
         <v>887</v>
       </c>
-      <c r="D243" s="4" t="s">
+      <c r="D243" s="2" t="s">
         <v>888</v>
       </c>
       <c r="E243" s="1" t="s">
@@ -13923,7 +13914,7 @@
       <c r="C244" s="1" t="s">
         <v>890</v>
       </c>
-      <c r="D244" s="4" t="s">
+      <c r="D244" s="2" t="s">
         <v>891</v>
       </c>
       <c r="E244" s="1" t="s">
@@ -13947,7 +13938,7 @@
       <c r="C245" s="1" t="s">
         <v>893</v>
       </c>
-      <c r="D245" s="4" t="s">
+      <c r="D245" s="2" t="s">
         <v>894</v>
       </c>
       <c r="E245" s="1" t="s">
@@ -13973,7 +13964,7 @@
       <c r="C246" s="1" t="s">
         <v>884</v>
       </c>
-      <c r="D246" s="4" t="s">
+      <c r="D246" s="2" t="s">
         <v>898</v>
       </c>
       <c r="E246" s="1" t="s">
@@ -13999,7 +13990,7 @@
       <c r="C247" s="1" t="s">
         <v>887</v>
       </c>
-      <c r="D247" s="4" t="s">
+      <c r="D247" s="2" t="s">
         <v>902</v>
       </c>
       <c r="E247" s="1" t="s">
@@ -14025,7 +14016,7 @@
       <c r="C248" s="1" t="s">
         <v>890</v>
       </c>
-      <c r="D248" s="4" t="s">
+      <c r="D248" s="2" t="s">
         <v>906</v>
       </c>
       <c r="E248" s="1" t="s">
@@ -14051,7 +14042,7 @@
       <c r="C249" s="1" t="s">
         <v>890</v>
       </c>
-      <c r="D249" s="4" t="s">
+      <c r="D249" s="2" t="s">
         <v>910</v>
       </c>
       <c r="E249" s="1" t="s">
@@ -14077,7 +14068,7 @@
       <c r="C250" s="1" t="s">
         <v>914</v>
       </c>
-      <c r="D250" s="4" t="s">
+      <c r="D250" s="2" t="s">
         <v>3</v>
       </c>
       <c r="E250" s="1" t="s">
@@ -14101,7 +14092,7 @@
       <c r="C251" s="1" t="s">
         <v>916</v>
       </c>
-      <c r="D251" s="4" t="s">
+      <c r="D251" s="2" t="s">
         <v>917</v>
       </c>
       <c r="E251" s="1" t="s">
@@ -14127,7 +14118,7 @@
       <c r="C252" s="1" t="s">
         <v>921</v>
       </c>
-      <c r="D252" s="4" t="s">
+      <c r="D252" s="2" t="s">
         <v>922</v>
       </c>
       <c r="E252" s="1" t="s">
@@ -14153,7 +14144,7 @@
       <c r="C253" s="1" t="s">
         <v>926</v>
       </c>
-      <c r="D253" s="4" t="s">
+      <c r="D253" s="2" t="s">
         <v>927</v>
       </c>
       <c r="E253" s="1" t="s">
@@ -14179,7 +14170,7 @@
       <c r="C254" s="1" t="s">
         <v>931</v>
       </c>
-      <c r="D254" s="4" t="s">
+      <c r="D254" s="2" t="s">
         <v>932</v>
       </c>
       <c r="E254" s="1" t="s">
@@ -14205,7 +14196,7 @@
       <c r="C255" s="1" t="s">
         <v>936</v>
       </c>
-      <c r="D255" s="4" t="s">
+      <c r="D255" s="2" t="s">
         <v>937</v>
       </c>
       <c r="E255" s="1" t="s">
@@ -14231,7 +14222,7 @@
       <c r="C256" s="1" t="s">
         <v>941</v>
       </c>
-      <c r="D256" s="4" t="s">
+      <c r="D256" s="2" t="s">
         <v>942</v>
       </c>
       <c r="E256" s="1" t="s">
@@ -14257,7 +14248,7 @@
       <c r="C257" s="1" t="s">
         <v>946</v>
       </c>
-      <c r="D257" s="4" t="s">
+      <c r="D257" s="2" t="s">
         <v>947</v>
       </c>
       <c r="E257" s="1" t="s">
@@ -14283,7 +14274,7 @@
       <c r="C258" s="1" t="s">
         <v>951</v>
       </c>
-      <c r="D258" s="4" t="s">
+      <c r="D258" s="2" t="s">
         <v>952</v>
       </c>
       <c r="E258" s="1" t="s">
@@ -14309,7 +14300,7 @@
       <c r="C259" s="1" t="s">
         <v>956</v>
       </c>
-      <c r="D259" s="4" t="s">
+      <c r="D259" s="2" t="s">
         <v>957</v>
       </c>
       <c r="E259" s="1" t="s">
@@ -14335,7 +14326,7 @@
       <c r="C260" s="1" t="s">
         <v>961</v>
       </c>
-      <c r="D260" s="4" t="s">
+      <c r="D260" s="2" t="s">
         <v>962</v>
       </c>
       <c r="E260" s="1" t="s">
@@ -14361,7 +14352,7 @@
       <c r="C261" s="1" t="s">
         <v>966</v>
       </c>
-      <c r="D261" s="4" t="s">
+      <c r="D261" s="2" t="s">
         <v>967</v>
       </c>
       <c r="E261" s="1" t="s">
@@ -14387,7 +14378,7 @@
       <c r="C262" s="1" t="s">
         <v>971</v>
       </c>
-      <c r="D262" s="4" t="s">
+      <c r="D262" s="2" t="s">
         <v>972</v>
       </c>
       <c r="E262" s="1" t="s">
@@ -14413,7 +14404,7 @@
       <c r="C263" s="1" t="s">
         <v>976</v>
       </c>
-      <c r="D263" s="4" t="s">
+      <c r="D263" s="2" t="s">
         <v>977</v>
       </c>
       <c r="E263" s="1" t="s">
@@ -14439,7 +14430,7 @@
       <c r="C264" s="1" t="s">
         <v>981</v>
       </c>
-      <c r="D264" s="4" t="s">
+      <c r="D264" s="2" t="s">
         <v>982</v>
       </c>
       <c r="E264" s="1" t="s">
@@ -14465,7 +14456,7 @@
       <c r="C265" s="1" t="s">
         <v>986</v>
       </c>
-      <c r="D265" s="4" t="s">
+      <c r="D265" s="2" t="s">
         <v>987</v>
       </c>
       <c r="E265" s="1" t="s">
@@ -14491,7 +14482,7 @@
       <c r="C266" s="1" t="s">
         <v>991</v>
       </c>
-      <c r="D266" s="4" t="s">
+      <c r="D266" s="2" t="s">
         <v>992</v>
       </c>
       <c r="E266" s="1" t="s">
@@ -14517,7 +14508,7 @@
       <c r="C267" s="1" t="s">
         <v>996</v>
       </c>
-      <c r="D267" s="4" t="s">
+      <c r="D267" s="2" t="s">
         <v>997</v>
       </c>
       <c r="E267" s="1" t="s">
@@ -14543,7 +14534,7 @@
       <c r="C268" s="1" t="s">
         <v>1001</v>
       </c>
-      <c r="D268" s="4" t="s">
+      <c r="D268" s="2" t="s">
         <v>1002</v>
       </c>
       <c r="E268" s="1" t="s">
@@ -14569,7 +14560,7 @@
       <c r="C269" s="1" t="s">
         <v>1006</v>
       </c>
-      <c r="D269" s="4" t="s">
+      <c r="D269" s="2" t="s">
         <v>1007</v>
       </c>
       <c r="E269" s="1" t="s">
@@ -14595,7 +14586,7 @@
       <c r="C270" s="1" t="s">
         <v>1011</v>
       </c>
-      <c r="D270" s="4" t="s">
+      <c r="D270" s="2" t="s">
         <v>1012</v>
       </c>
       <c r="E270" s="1" t="s">
@@ -14621,7 +14612,7 @@
       <c r="C271" s="1" t="s">
         <v>1015</v>
       </c>
-      <c r="D271" s="4" t="s">
+      <c r="D271" s="2" t="s">
         <v>1016</v>
       </c>
       <c r="E271" s="1" t="s">
@@ -14647,7 +14638,7 @@
       <c r="C272" s="1" t="s">
         <v>1020</v>
       </c>
-      <c r="D272" s="4" t="s">
+      <c r="D272" s="2" t="s">
         <v>1021</v>
       </c>
       <c r="E272" s="1" t="s">
@@ -14673,7 +14664,7 @@
       <c r="C273" s="1" t="s">
         <v>1025</v>
       </c>
-      <c r="D273" s="4" t="s">
+      <c r="D273" s="2" t="s">
         <v>1026</v>
       </c>
       <c r="E273" s="1" t="s">
@@ -14699,7 +14690,7 @@
       <c r="C274" s="1" t="s">
         <v>887</v>
       </c>
-      <c r="D274" s="4" t="s">
+      <c r="D274" s="2" t="s">
         <v>1030</v>
       </c>
       <c r="E274" s="1" t="s">
@@ -14725,7 +14716,7 @@
       <c r="C275" s="1" t="s">
         <v>887</v>
       </c>
-      <c r="D275" s="4" t="s">
+      <c r="D275" s="2" t="s">
         <v>1034</v>
       </c>
       <c r="E275" s="1" t="s">
@@ -14751,7 +14742,7 @@
       <c r="C276" s="1" t="s">
         <v>1038</v>
       </c>
-      <c r="D276" s="4" t="s">
+      <c r="D276" s="2" t="s">
         <v>1039</v>
       </c>
       <c r="E276" s="1" t="s">
@@ -14777,7 +14768,7 @@
       <c r="C277" s="1" t="s">
         <v>1043</v>
       </c>
-      <c r="D277" s="4" t="s">
+      <c r="D277" s="2" t="s">
         <v>1044</v>
       </c>
       <c r="E277" s="1" t="s">
@@ -14801,7 +14792,7 @@
       <c r="C278" s="1" t="s">
         <v>1048</v>
       </c>
-      <c r="D278" s="4" t="s">
+      <c r="D278" s="2" t="s">
         <v>1049</v>
       </c>
       <c r="E278" s="1" t="s">
@@ -14823,7 +14814,7 @@
       <c r="C279" s="1" t="s">
         <v>1051</v>
       </c>
-      <c r="D279" s="4" t="s">
+      <c r="D279" s="2" t="s">
         <v>1052</v>
       </c>
       <c r="E279" s="1" t="s">
@@ -14847,7 +14838,7 @@
       <c r="C280" s="1" t="s">
         <v>1055</v>
       </c>
-      <c r="D280" s="4" t="s">
+      <c r="D280" s="2" t="s">
         <v>1056</v>
       </c>
       <c r="E280" s="1" t="s">
@@ -14873,7 +14864,7 @@
       <c r="C281" s="1" t="s">
         <v>1060</v>
       </c>
-      <c r="D281" s="4" t="s">
+      <c r="D281" s="2" t="s">
         <v>1061</v>
       </c>
       <c r="E281" s="1" t="s">
@@ -14899,7 +14890,7 @@
       <c r="C282" s="1" t="s">
         <v>1065</v>
       </c>
-      <c r="D282" s="4" t="s">
+      <c r="D282" s="2" t="s">
         <v>1066</v>
       </c>
       <c r="E282" s="1" t="s">
@@ -14925,7 +14916,7 @@
       <c r="C283" s="1" t="s">
         <v>1070</v>
       </c>
-      <c r="D283" s="4" t="s">
+      <c r="D283" s="2" t="s">
         <v>1071</v>
       </c>
       <c r="E283" s="1" t="s">
@@ -14951,7 +14942,7 @@
       <c r="C284" s="1" t="s">
         <v>1075</v>
       </c>
-      <c r="D284" s="4" t="s">
+      <c r="D284" s="2" t="s">
         <v>1076</v>
       </c>
       <c r="E284" s="1" t="s">
@@ -14977,7 +14968,7 @@
       <c r="C285" s="1" t="s">
         <v>1080</v>
       </c>
-      <c r="D285" s="4" t="s">
+      <c r="D285" s="2" t="s">
         <v>1081</v>
       </c>
       <c r="E285" s="1" t="s">
@@ -15003,7 +14994,7 @@
       <c r="C286" s="1" t="s">
         <v>1085</v>
       </c>
-      <c r="D286" s="4" t="s">
+      <c r="D286" s="2" t="s">
         <v>1086</v>
       </c>
       <c r="E286" s="1" t="s">
@@ -15027,7 +15018,7 @@
       <c r="C287" s="1" t="s">
         <v>1089</v>
       </c>
-      <c r="D287" s="4" t="s">
+      <c r="D287" s="2" t="s">
         <v>1090</v>
       </c>
       <c r="E287" s="1" t="s">
@@ -15053,7 +15044,7 @@
       <c r="C288" s="1" t="s">
         <v>1094</v>
       </c>
-      <c r="D288" s="4" t="s">
+      <c r="D288" s="2" t="s">
         <v>1095</v>
       </c>
       <c r="E288" s="1" t="s">
@@ -15079,7 +15070,7 @@
       <c r="C289" s="1" t="s">
         <v>1099</v>
       </c>
-      <c r="D289" s="4" t="s">
+      <c r="D289" s="2" t="s">
         <v>1100</v>
       </c>
       <c r="E289" s="1" t="s">
@@ -15105,7 +15096,7 @@
       <c r="C290" s="1" t="s">
         <v>1104</v>
       </c>
-      <c r="D290" s="4" t="s">
+      <c r="D290" s="2" t="s">
         <v>1105</v>
       </c>
       <c r="E290" s="1" t="s">
@@ -15131,7 +15122,7 @@
       <c r="C291" s="1" t="s">
         <v>1109</v>
       </c>
-      <c r="D291" s="5" t="s">
+      <c r="D291" s="3" t="s">
         <v>3</v>
       </c>
       <c r="E291" s="1" t="s">
@@ -15153,7 +15144,7 @@
       <c r="C292" s="1" t="s">
         <v>1111</v>
       </c>
-      <c r="D292" s="5" t="s">
+      <c r="D292" s="3" t="s">
         <v>3</v>
       </c>
       <c r="E292" s="1" t="s">

</xml_diff>